<commit_message>
diagnosis_history 테이블 명세서 수정
</commit_message>
<xml_diff>
--- a/diagnosis_history 테이블 명세서.xlsx
+++ b/diagnosis_history 테이블 명세서.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\myrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Table Specification</t>
   </si>
@@ -634,6 +634,14 @@
   </si>
   <si>
     <t>diagnosis_definition</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>medicine</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상비약</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -654,6 +662,8 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -755,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -982,6 +992,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -989,16 +1012,86 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1008,9 +1101,11 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1019,54 +1114,13 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1077,7 +1131,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1117,14 +1171,89 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1138,128 +1267,74 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1542,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L23"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1557,209 +1632,209 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="20"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="20"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="20"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="20"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="20"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="20"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="31">
+      <c r="B11" s="14">
         <v>1</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38" t="s">
+      <c r="D11" s="51"/>
+      <c r="E11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="17">
         <v>20</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40" t="s">
+      <c r="I11" s="18"/>
+      <c r="J11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="42" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="31">
+      <c r="B12" s="14">
         <v>2</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1773,20 +1848,20 @@
         <v>24</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="13" t="s">
         <v>48</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="44"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="31">
+      <c r="B13" s="14">
         <v>3</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="5" t="s">
         <v>42</v>
       </c>
@@ -1798,16 +1873,16 @@
         <v>49</v>
       </c>
       <c r="K13" s="7"/>
-      <c r="L13" s="45"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="31">
+      <c r="B14" s="14">
         <v>4</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="5" t="s">
         <v>43</v>
       </c>
@@ -1821,18 +1896,18 @@
         <v>50</v>
       </c>
       <c r="K14" s="7"/>
-      <c r="L14" s="45" t="s">
+      <c r="L14" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="31">
+      <c r="B15" s="14">
         <v>5</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="5" t="s">
         <v>42</v>
       </c>
@@ -1844,16 +1919,16 @@
         <v>51</v>
       </c>
       <c r="K15" s="7"/>
-      <c r="L15" s="45"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="31">
+      <c r="B16" s="14">
         <v>6</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="5" t="s">
         <v>42</v>
       </c>
@@ -1865,16 +1940,16 @@
         <v>52</v>
       </c>
       <c r="K16" s="7"/>
-      <c r="L16" s="45"/>
+      <c r="L16" s="23"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="31">
+      <c r="B17" s="14">
         <v>7</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="5" t="s">
         <v>42</v>
       </c>
@@ -1886,16 +1961,16 @@
         <v>53</v>
       </c>
       <c r="K17" s="7"/>
-      <c r="L17" s="45"/>
+      <c r="L17" s="23"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="31">
+      <c r="B18" s="14">
         <v>8</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="5" t="s">
         <v>42</v>
       </c>
@@ -1909,130 +1984,154 @@
         <v>54</v>
       </c>
       <c r="K18" s="7"/>
-      <c r="L18" s="45"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="31">
+      <c r="B19" s="54">
         <v>9</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="48" t="s">
+      <c r="D19" s="56"/>
+      <c r="E19" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53" t="s">
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="49"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="26"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="20"/>
+      <c r="B20" s="63">
+        <v>10</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="25"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C22" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="2" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G22" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="59" t="s">
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="58"/>
-    </row>
-    <row r="22" spans="2:12">
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="K22" s="56"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" s="33"/>
+      <c r="L23" s="34"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C24" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="5" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G24" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="56" t="s">
+      <c r="H24" s="29"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
+  <mergeCells count="36">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:L4"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:L9"/>
@@ -2043,20 +2142,18 @@
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:L7"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>